<commit_message>
Removed IS, tried removing TEL derrivative, but worsened model, reverted to IS but fixed C value for SVM
</commit_message>
<xml_diff>
--- a/output_summary_combined_models_interpretation.xlsx
+++ b/output_summary_combined_models_interpretation.xlsx
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98.5</v>
+        <v>99.3</v>
       </c>
       <c r="D2" t="n">
-        <v>21.9</v>
+        <v>18.9</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -495,10 +495,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>71.3</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>86.8</v>
+        <v>86.09999999999999</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>

</xml_diff>